<commit_message>
Nueva columna de idOrganizacion y mejora de ALMACEN
</commit_message>
<xml_diff>
--- a/BASE DE DATOS TODO NEGOCIO.xlsx
+++ b/BASE DE DATOS TODO NEGOCIO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\TODO-NEGOCIO-FRONT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D78EE8E-9FE8-4F9B-9789-B89E6C3BA510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2094AA7-80F7-480B-9541-A074F2D1C9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-84" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLAS" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -754,67 +748,67 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1519,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2578A653-945C-4D88-8D61-A7A3860A5136}">
   <dimension ref="A4:U82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S79" sqref="S79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,21 +1541,23 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="K4" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="9"/>
+      <c r="K4" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="9"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -1739,22 +1735,25 @@
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="H13" s="38" t="s">
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="9"/>
+      <c r="H13" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-      <c r="M13" s="39" t="s">
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="9"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
@@ -1788,12 +1787,12 @@
         <v>87</v>
       </c>
       <c r="Q14" s="9"/>
-      <c r="R14" s="31" t="s">
+      <c r="R14" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="S14" s="31"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
+      <c r="S14" s="39"/>
+      <c r="T14" s="39"/>
+      <c r="U14" s="39"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
@@ -1952,21 +1951,22 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="9"/>
-      <c r="H22" s="41" t="s">
+      <c r="H22" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="43"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="9"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
@@ -2050,21 +2050,23 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="N30" s="32" t="s">
+      <c r="N30" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="O30" s="32"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="32"/>
-      <c r="R30" s="32"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="40"/>
+      <c r="R30" s="40"/>
+      <c r="S30" s="9"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F31" s="33" t="s">
+      <c r="F31" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="9"/>
       <c r="N31" s="2" t="s">
         <v>26</v>
       </c>
@@ -2111,7 +2113,7 @@
       </c>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F33" s="2">
         <v>1</v>
       </c>
@@ -2141,7 +2143,7 @@
       </c>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F34" s="2">
         <v>1</v>
       </c>
@@ -2171,7 +2173,7 @@
       </c>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F35" s="2">
         <v>1</v>
       </c>
@@ -2201,7 +2203,7 @@
       </c>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F36" s="2">
         <v>1</v>
       </c>
@@ -2231,7 +2233,7 @@
       </c>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F37" s="2">
         <v>1</v>
       </c>
@@ -2261,7 +2263,7 @@
       </c>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F38" s="2">
         <v>1</v>
       </c>
@@ -2291,7 +2293,7 @@
       </c>
       <c r="S38" s="1"/>
     </row>
-    <row r="39" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F39" s="2">
         <v>1</v>
       </c>
@@ -2321,7 +2323,7 @@
       </c>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F40" s="2">
         <v>1</v>
       </c>
@@ -2335,17 +2337,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="K44" s="44" t="s">
+    <row r="44" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="K44" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="L44" s="44"/>
-      <c r="M44" s="44"/>
-      <c r="N44" s="44"/>
-      <c r="O44" s="44"/>
-      <c r="P44" s="44"/>
-    </row>
-    <row r="45" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="L44" s="35"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="35"/>
+      <c r="O44" s="35"/>
+      <c r="P44" s="35"/>
+      <c r="Q44" s="9"/>
+    </row>
+    <row r="45" spans="6:20" x14ac:dyDescent="0.25">
       <c r="K45" s="2" t="s">
         <v>52</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:20" x14ac:dyDescent="0.25">
       <c r="K46" s="11">
         <v>1</v>
       </c>
@@ -2385,12 +2388,13 @@
         <v>134</v>
       </c>
     </row>
-    <row r="47" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="G47" s="34" t="s">
+    <row r="47" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="G47" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="25"/>
+      <c r="J47" s="9"/>
       <c r="K47" s="13">
         <v>2</v>
       </c>
@@ -2409,12 +2413,13 @@
       <c r="P47" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="R47" s="30" t="s">
+      <c r="R47" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="S47" s="30"/>
-    </row>
-    <row r="48" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="S47" s="37"/>
+      <c r="T47" s="9"/>
+    </row>
+    <row r="48" spans="6:20" x14ac:dyDescent="0.25">
       <c r="G48" s="2" t="s">
         <v>55</v>
       </c>
@@ -2526,12 +2531,13 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
-      <c r="R54" s="29" t="s">
+      <c r="Q54" s="9"/>
+      <c r="R54" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="S54" s="29"/>
-      <c r="T54" s="29"/>
-      <c r="U54" s="29"/>
+      <c r="S54" s="36"/>
+      <c r="T54" s="36"/>
+      <c r="U54" s="36"/>
     </row>
     <row r="55" spans="7:21" x14ac:dyDescent="0.25">
       <c r="R55" s="2" t="s">
@@ -2562,14 +2568,16 @@
       </c>
     </row>
     <row r="57" spans="7:21" x14ac:dyDescent="0.25">
-      <c r="K57" s="27" t="s">
+      <c r="K57" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="L57" s="27"/>
-      <c r="N57" s="28" t="s">
+      <c r="L57" s="43"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="O57" s="28"/>
+      <c r="O57" s="44"/>
+      <c r="P57" s="9"/>
       <c r="R57" s="3">
         <v>2</v>
       </c>
@@ -2632,15 +2640,16 @@
       </c>
     </row>
     <row r="63" spans="7:21" x14ac:dyDescent="0.25">
-      <c r="K63" s="26" t="s">
+      <c r="K63" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="L63" s="26"/>
-      <c r="M63" s="26"/>
-      <c r="N63" s="26"/>
-      <c r="O63" s="26"/>
-      <c r="P63" s="26"/>
-      <c r="Q63" s="26"/>
+      <c r="L63" s="38"/>
+      <c r="M63" s="38"/>
+      <c r="N63" s="38"/>
+      <c r="O63" s="38"/>
+      <c r="P63" s="38"/>
+      <c r="Q63" s="38"/>
+      <c r="R63" s="9"/>
     </row>
     <row r="64" spans="7:21" x14ac:dyDescent="0.25">
       <c r="K64" s="2" t="s">
@@ -2665,7 +2674,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:19" x14ac:dyDescent="0.25">
       <c r="K65" s="11">
         <v>1</v>
       </c>
@@ -2689,11 +2698,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H66" s="24" t="s">
+    <row r="66" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H66" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="I66" s="24"/>
+      <c r="I66" s="41"/>
+      <c r="J66" s="9"/>
       <c r="K66" s="11">
         <v>2</v>
       </c>
@@ -2717,7 +2727,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H67" s="2" t="s">
         <v>77</v>
       </c>
@@ -2747,7 +2757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H68" s="2">
         <v>1</v>
       </c>
@@ -2777,7 +2787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
       <c r="K69" s="8">
@@ -2803,13 +2813,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H75" s="25" t="s">
+    <row r="75" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H75" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="I75" s="25"/>
-    </row>
-    <row r="76" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="I75" s="42"/>
+      <c r="J75" s="9"/>
+    </row>
+    <row r="76" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H76" s="2" t="s">
         <v>131</v>
       </c>
@@ -2817,7 +2828,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="77" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H77" s="2">
         <v>1</v>
       </c>
@@ -2825,7 +2836,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="78" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H78" s="2">
         <v>2</v>
       </c>
@@ -2833,25 +2844,26 @@
         <v>141</v>
       </c>
     </row>
-    <row r="79" spans="8:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:19" x14ac:dyDescent="0.25">
       <c r="H79" s="2">
         <v>3</v>
       </c>
       <c r="I79" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="K79" s="26" t="s">
+      <c r="K79" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="L79" s="26"/>
-      <c r="M79" s="26"/>
-      <c r="N79" s="26"/>
-      <c r="O79" s="26"/>
-      <c r="P79" s="26"/>
-      <c r="Q79" s="26"/>
-      <c r="R79" s="26"/>
-    </row>
-    <row r="80" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="L79" s="38"/>
+      <c r="M79" s="38"/>
+      <c r="N79" s="38"/>
+      <c r="O79" s="38"/>
+      <c r="P79" s="38"/>
+      <c r="Q79" s="38"/>
+      <c r="R79" s="38"/>
+      <c r="S79" s="9"/>
+    </row>
+    <row r="80" spans="8:19" x14ac:dyDescent="0.25">
       <c r="K80" s="3" t="s">
         <v>52</v>
       </c>
@@ -2929,6 +2941,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="K79:R79"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="N57:O57"/>
+    <mergeCell ref="R54:U54"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="K63:Q63"/>
+    <mergeCell ref="R14:U14"/>
+    <mergeCell ref="N30:R30"/>
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="G47:I47"/>
     <mergeCell ref="B4:H4"/>
@@ -2939,16 +2961,6 @@
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="H22:L22"/>
     <mergeCell ref="K44:P44"/>
-    <mergeCell ref="R54:U54"/>
-    <mergeCell ref="R47:S47"/>
-    <mergeCell ref="K63:Q63"/>
-    <mergeCell ref="R14:U14"/>
-    <mergeCell ref="N30:R30"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="K79:R79"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="N57:O57"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" xr:uid="{F36046BF-2A29-4391-BBF2-8E3D47387CCC}"/>

</xml_diff>